<commit_message>
adjusted arff creating file for tests
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -3,29 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D977A35F-C432-427C-802E-85E7C27C782E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BD843F-0A12-4D89-BAAC-5210A71C1244}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="nltkClassifier" sheetId="1" r:id="rId1"/>
+    <sheet name="Ideen" sheetId="2" r:id="rId2"/>
+    <sheet name="Accuracy" sheetId="3" r:id="rId3"/>
+    <sheet name="ClassifierOutput" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Accuracy!$A$1:$B$26</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
   <si>
     <t>NaiveBayes</t>
   </si>
@@ -43,6 +44,279 @@
   </si>
   <si>
     <t>DecisionTree</t>
+  </si>
+  <si>
+    <t>Konfigurationen</t>
+  </si>
+  <si>
+    <t>mit/ohne Stopwords</t>
+  </si>
+  <si>
+    <t>Topwords-Threshold</t>
+  </si>
+  <si>
+    <t>Stemming</t>
+  </si>
+  <si>
+    <t>rules.ZeroR</t>
+  </si>
+  <si>
+    <t>rules.JRip</t>
+  </si>
+  <si>
+    <t>rules.DecisionTable</t>
+  </si>
+  <si>
+    <t>bayes.NaiveBayes</t>
+  </si>
+  <si>
+    <t>bayes.NaiveBayesMultinomial</t>
+  </si>
+  <si>
+    <t>bayes.NaiveBayesMultinomialText</t>
+  </si>
+  <si>
+    <t>trees.RandomForest</t>
+  </si>
+  <si>
+    <t>trees.RandomTree</t>
+  </si>
+  <si>
+    <t>Cross-validation (10 Folds)</t>
+  </si>
+  <si>
+    <t>bayes.BayesNet</t>
+  </si>
+  <si>
+    <t>Weitere Features</t>
+  </si>
+  <si>
+    <t>trees.REPTree</t>
+  </si>
+  <si>
+    <t>trees.J48</t>
+  </si>
+  <si>
+    <t>bayes.NaiveBayesUpdateable</t>
+  </si>
+  <si>
+    <t>bayes.NaiveBayesMultinomialUpdateable</t>
+  </si>
+  <si>
+    <t>trees.DecisionStump</t>
+  </si>
+  <si>
+    <t>trees.HoeffdingTree</t>
+  </si>
+  <si>
+    <t>trees.LMT</t>
+  </si>
+  <si>
+    <t>rules.OneR</t>
+  </si>
+  <si>
+    <t>rules.PART</t>
+  </si>
+  <si>
+    <t>meta.AdaBoostM1</t>
+  </si>
+  <si>
+    <t>meta.AttributeSelectedClassifier</t>
+  </si>
+  <si>
+    <t>mehr als zwei Klassen</t>
+  </si>
+  <si>
+    <t>meta.Bagging</t>
+  </si>
+  <si>
+    <t>meta.ClassificationViaRegression</t>
+  </si>
+  <si>
+    <t>meta.CVParameterSelection</t>
+  </si>
+  <si>
+    <t>meta.FilteredClassifier</t>
+  </si>
+  <si>
+    <t>functions.Logistic</t>
+  </si>
+  <si>
+    <t>functions.SGD</t>
+  </si>
+  <si>
+    <t>functions.SGDText</t>
+  </si>
+  <si>
+    <t>functions.SimpleLogistic</t>
+  </si>
+  <si>
+    <t>functions.SMO</t>
+  </si>
+  <si>
+    <t>functions.VotedPerceptron</t>
+  </si>
+  <si>
+    <t>functions.MultilayerPerceptron</t>
+  </si>
+  <si>
+    <t>lazy.Ibk</t>
+  </si>
+  <si>
+    <t>lazy.Kstar</t>
+  </si>
+  <si>
+    <t>lazy.LWL</t>
+  </si>
+  <si>
+    <t>meta.IterativeClassifierOptimizer</t>
+  </si>
+  <si>
+    <t>meta.LogitBoost</t>
+  </si>
+  <si>
+    <t>meta.MultiClassClassifier</t>
+  </si>
+  <si>
+    <t>meta.MultiClassClassifierUpdateable</t>
+  </si>
+  <si>
+    <t>meta.MultiScheme</t>
+  </si>
+  <si>
+    <t>meta.RandomCommittee</t>
+  </si>
+  <si>
+    <t>meta.RandomizableFilteredClassifier</t>
+  </si>
+  <si>
+    <t>meta.RandomSubSpace</t>
+  </si>
+  <si>
+    <t>meta.Stacking</t>
+  </si>
+  <si>
+    <t>meta.Vote</t>
+  </si>
+  <si>
+    <t>meta.WeightedInstancesHandlerWrapper</t>
+  </si>
+  <si>
+    <t>100, no stopwords</t>
+  </si>
+  <si>
+    <t>100, with stopwords</t>
+  </si>
+  <si>
+    <t>1000, no stopwords</t>
+  </si>
+  <si>
+    <t>1000, with stopwords</t>
+  </si>
+  <si>
+    <t>all, without stopwords</t>
+  </si>
+  <si>
+    <t>TFIDF Vectorizer</t>
+  </si>
+  <si>
+    <t>Lowercase</t>
+  </si>
+  <si>
+    <t>heaperror</t>
+  </si>
+  <si>
+    <t>=== Run information ===</t>
+  </si>
+  <si>
+    <t>Scheme:       weka.classifiers.trees.RandomForest -P 100 -I 100 -num-slots 1 -K 0 -M 1.0 -V 0.001 -S 1</t>
+  </si>
+  <si>
+    <t>Relation:     comment</t>
+  </si>
+  <si>
+    <t>Instances:    4659</t>
+  </si>
+  <si>
+    <t>Attributes:   9937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              [list of attributes omitted]</t>
+  </si>
+  <si>
+    <t>Test mode:    10-fold cross-validation</t>
+  </si>
+  <si>
+    <t>=== Classifier model (full training set) ===</t>
+  </si>
+  <si>
+    <t>RandomForest</t>
+  </si>
+  <si>
+    <t>Bagging with 100 iterations and base learner</t>
+  </si>
+  <si>
+    <t>weka.classifiers.trees.RandomTree -K 0 -M 1.0 -V 0.001 -S 1 -do-not-check-capabilities</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 344.52 seconds</t>
+  </si>
+  <si>
+    <t>=== Stratified cross-validation ===</t>
+  </si>
+  <si>
+    <t>=== Summary ===</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances        3708               79.5879 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances       951               20.4121 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.3855</t>
+  </si>
+  <si>
+    <t>Mean absolute error                      0.3055</t>
+  </si>
+  <si>
+    <t>Root mean squared error                  0.3872</t>
+  </si>
+  <si>
+    <t>Relative absolute error                 77.0532 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             86.9737 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Number of Instances             4659     </t>
+  </si>
+  <si>
+    <t>=== Detailed Accuracy By Class ===</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 TP Rate  FP Rate  Precision  Recall   F-Measure  MCC      ROC Area  PRC Area  Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,957    0,634    0,801      0,957    0,872      0,426    0,782     0,889     True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,366    0,043    0,760      0,366    0,494      0,426    0,782     0,645     False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Avg.    0,796    0,473    0,790      0,796    0,769      0,426    0,782     0,823     </t>
+  </si>
+  <si>
+    <t>=== Confusion Matrix ===</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a    b   &lt;-- classified as</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3243  147 |    a = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  804  465 |    b = False</t>
   </si>
 </sst>
 </file>
@@ -58,12 +332,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,12 +358,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -366,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -375,18 +657,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -545,43 +827,43 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <f>(B2+B5)/SUM(B2:B5)</f>
         <v>0.7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f>(C2+C5)/SUM(C2:C5)</f>
         <v>0.74285714285714288</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <f t="shared" ref="D6:K6" si="1">(D2+D5)/SUM(D2:D5)</f>
         <v>0.47142857142857142</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f t="shared" si="1"/>
         <v>0.62857142857142856</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f t="shared" si="1"/>
         <v>0.61428571428571432</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f t="shared" si="1"/>
         <v>0.67142857142857137</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <f t="shared" si="1"/>
         <v>0.65714285714285714</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <f t="shared" si="1"/>
         <v>0.65714285714285714</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <f t="shared" si="1"/>
         <v>0.52857142857142858</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -591,43 +873,43 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <f>MAX((B2+B3)/SUM(B2:B5),1-(B2+B3)/SUM(B2:B5))</f>
         <v>0.61428571428571432</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f>MAX((C2+C3)/SUM(C2:C5),1-(C2+C3)/SUM(C2:C5))</f>
         <v>0.5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <f t="shared" ref="D7:K7" si="2">MAX((D2+D3)/SUM(D2:D5),1-(D2+D3)/SUM(D2:D5))</f>
         <v>0.61428571428571432</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
         <v>0.52857142857142858</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f t="shared" si="2"/>
         <v>0.58571428571428574</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <f t="shared" si="2"/>
         <v>0.51428571428571423</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f t="shared" si="2"/>
         <v>0.51428571428571423</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <f t="shared" si="2"/>
         <v>0.51428571428571423</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <f t="shared" si="2"/>
         <v>0.51428571428571423</v>
       </c>
@@ -637,18 +919,18 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -807,43 +1089,43 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <f>(B10+B13)/SUM(B10:B13)</f>
         <v>0.67142857142857137</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <f>(C10+C13)/SUM(C10:C13)</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <f t="shared" ref="D14" si="4">(D10+D13)/SUM(D10:D13)</f>
         <v>0.7</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <f t="shared" ref="E14" si="5">(E10+E13)/SUM(E10:E13)</f>
         <v>0.7</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <f t="shared" ref="F14" si="6">(F10+F13)/SUM(F10:F13)</f>
         <v>0.68571428571428572</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <f t="shared" ref="G14" si="7">(G10+G13)/SUM(G10:G13)</f>
         <v>0.62857142857142856</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <f t="shared" ref="H14" si="8">(H10+H13)/SUM(H10:H13)</f>
         <v>0.61428571428571432</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <f t="shared" ref="I14" si="9">(I10+I13)/SUM(I10:I13)</f>
         <v>0.68571428571428572</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <f t="shared" ref="J14" si="10">(J10+J13)/SUM(J10:J13)</f>
         <v>0.65714285714285714</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <f t="shared" ref="K14" si="11">(K10+K13)/SUM(K10:K13)</f>
         <v>0.61428571428571432</v>
       </c>
@@ -853,43 +1135,43 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <f>MAX((B10+B11)/SUM(B10:B13),1-(B10+B11)/SUM(B10:B13))</f>
         <v>0.58571428571428563</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f>MAX((C10+C11)/SUM(C10:C13),1-(C10+C11)/SUM(C10:C13))</f>
         <v>0.51428571428571423</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <f t="shared" ref="D15:K15" si="12">MAX((D10+D11)/SUM(D10:D13),1-(D10+D11)/SUM(D10:D13))</f>
         <v>0.52857142857142858</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <f t="shared" si="12"/>
         <v>0.55714285714285716</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <f t="shared" si="12"/>
         <v>0.52857142857142858</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <f t="shared" si="12"/>
         <v>0.51428571428571423</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <f t="shared" si="12"/>
         <v>0.51428571428571423</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <f t="shared" si="12"/>
         <v>0.55714285714285716</v>
       </c>
@@ -905,4 +1187,946 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74247B1C-FA49-495A-87B8-A1E34540CE36}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59F50FD-8FC7-422A-8F8D-928176239229}">
+  <dimension ref="A1:F46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.6328125" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="7.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>74.221900000000005</v>
+      </c>
+      <c r="C2">
+        <v>72.934100000000001</v>
+      </c>
+      <c r="D2">
+        <v>75.724400000000003</v>
+      </c>
+      <c r="E2">
+        <v>76.110799999999998</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>69.349599999999995</v>
+      </c>
+      <c r="C3">
+        <v>66.945700000000002</v>
+      </c>
+      <c r="D3">
+        <v>69.2423</v>
+      </c>
+      <c r="E3">
+        <v>67.031599999999997</v>
+      </c>
+      <c r="F3">
+        <v>69.177899999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>73.599500000000006</v>
+      </c>
+      <c r="C4">
+        <v>72.912599999999998</v>
+      </c>
+      <c r="D4">
+        <v>76.604399999999998</v>
+      </c>
+      <c r="E4">
+        <v>77.656099999999995</v>
+      </c>
+      <c r="F4">
+        <v>76.303899999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C5" s="2">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
+        <v>73.599500000000006</v>
+      </c>
+      <c r="C6" s="2">
+        <v>72.912599999999998</v>
+      </c>
+      <c r="D6">
+        <v>76.604399999999998</v>
+      </c>
+      <c r="E6">
+        <v>77.656099999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>69.349599999999995</v>
+      </c>
+      <c r="C7" s="2">
+        <v>66.945700000000002</v>
+      </c>
+      <c r="D7">
+        <v>69.2423</v>
+      </c>
+      <c r="E7">
+        <v>67.031599999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>73.363399999999999</v>
+      </c>
+      <c r="C8">
+        <v>73.556600000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>74.264899999999997</v>
+      </c>
+      <c r="C10">
+        <v>73.814099999999996</v>
+      </c>
+      <c r="D10">
+        <v>75.058999999999997</v>
+      </c>
+      <c r="E10">
+        <v>75.938999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C11" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="D11" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="E11" s="2">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>73.792699999999996</v>
+      </c>
+      <c r="C12">
+        <v>73.663899999999998</v>
+      </c>
+      <c r="D12">
+        <v>76.239500000000007</v>
+      </c>
+      <c r="E12">
+        <v>77.484399999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="C13">
+        <v>73.470699999999994</v>
+      </c>
+      <c r="D13">
+        <v>76.196600000000004</v>
+      </c>
+      <c r="E13">
+        <v>77.8279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>72.483400000000003</v>
+      </c>
+      <c r="C14">
+        <v>73.191699999999997</v>
+      </c>
+      <c r="D14">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="E14">
+        <v>75.102000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <v>71.667699999999996</v>
+      </c>
+      <c r="C15">
+        <v>70.337000000000003</v>
+      </c>
+      <c r="D15">
+        <v>71.946799999999996</v>
+      </c>
+      <c r="E15">
+        <v>71.946799999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>73.041399999999996</v>
+      </c>
+      <c r="C16">
+        <v>73.041399999999996</v>
+      </c>
+      <c r="D16">
+        <v>74.221900000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>73.492199999999997</v>
+      </c>
+      <c r="C17">
+        <v>72.783900000000003</v>
+      </c>
+      <c r="D17">
+        <v>73.449200000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>73.470699999999994</v>
+      </c>
+      <c r="C18">
+        <v>72.676500000000004</v>
+      </c>
+      <c r="D18">
+        <v>73.299000000000007</v>
+      </c>
+      <c r="E18">
+        <v>73.299000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>74.286299999999997</v>
+      </c>
+      <c r="C19">
+        <v>73.685299999999998</v>
+      </c>
+      <c r="D19">
+        <v>74.179000000000002</v>
+      </c>
+      <c r="E19">
+        <v>75.273700000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>74.436599999999999</v>
+      </c>
+      <c r="C20">
+        <v>73.663899999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C21">
+        <v>73.127300000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C22" s="2">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23">
+        <v>74.286299999999997</v>
+      </c>
+      <c r="C23">
+        <v>73.749700000000004</v>
+      </c>
+      <c r="D23">
+        <v>75.617099999999994</v>
+      </c>
+      <c r="E23">
+        <v>76.819100000000006</v>
+      </c>
+      <c r="F23">
+        <v>75.617099999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24">
+        <v>74.286299999999997</v>
+      </c>
+      <c r="C24">
+        <v>73.406300000000002</v>
+      </c>
+      <c r="D24">
+        <v>75.338099999999997</v>
+      </c>
+      <c r="E24">
+        <v>75.638499999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25">
+        <v>74.221900000000005</v>
+      </c>
+      <c r="C25">
+        <v>73.427800000000005</v>
+      </c>
+      <c r="D25">
+        <v>75.338099999999997</v>
+      </c>
+      <c r="E25">
+        <v>75.638499999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26">
+        <v>73.363399999999999</v>
+      </c>
+      <c r="C26">
+        <v>73.556600000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>74.264899999999997</v>
+      </c>
+      <c r="C27">
+        <v>73.814099999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C28" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="D28" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="E28" s="2">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29">
+        <v>72.504800000000003</v>
+      </c>
+      <c r="C29">
+        <v>73.857100000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30">
+        <v>69.929199999999994</v>
+      </c>
+      <c r="C30">
+        <v>68.791600000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31">
+        <v>73.449200000000005</v>
+      </c>
+      <c r="C31">
+        <v>73.620900000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C32" s="2">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C33" s="2">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="2">
+        <v>72.7624</v>
+      </c>
+      <c r="C34" s="2">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>74.393600000000006</v>
+      </c>
+      <c r="C35" s="3">
+        <v>73.556600000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>74.3078</v>
+      </c>
+      <c r="C36" s="3">
+        <v>73.105800000000002</v>
+      </c>
+      <c r="D36">
+        <v>75.423900000000003</v>
+      </c>
+      <c r="E36">
+        <v>74.415099999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>73.470699999999994</v>
+      </c>
+      <c r="C37" s="3">
+        <v>72.934100000000001</v>
+      </c>
+      <c r="D37">
+        <v>73.470699999999994</v>
+      </c>
+      <c r="E37">
+        <v>73.213099999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38">
+        <v>73.492199999999997</v>
+      </c>
+      <c r="C38" s="3">
+        <v>72.118499999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39">
+        <v>72.7624</v>
+      </c>
+      <c r="C39">
+        <v>72.7624</v>
+      </c>
+      <c r="D39">
+        <v>72.7624</v>
+      </c>
+      <c r="E39">
+        <v>72.7624</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40">
+        <v>73.470699999999994</v>
+      </c>
+      <c r="C40">
+        <v>72.676500000000004</v>
+      </c>
+      <c r="D40">
+        <v>73.299000000000007</v>
+      </c>
+      <c r="E40">
+        <v>73.299000000000007</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>73.256100000000004</v>
+      </c>
+      <c r="C41">
+        <v>73.062899999999999</v>
+      </c>
+      <c r="D41">
+        <v>72.719499999999996</v>
+      </c>
+      <c r="E41">
+        <v>72.633600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42">
+        <v>73.857100000000003</v>
+      </c>
+      <c r="C42">
+        <v>72.676500000000004</v>
+      </c>
+      <c r="D42">
+        <v>74.114599999999996</v>
+      </c>
+      <c r="E42">
+        <v>74.758499999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43">
+        <v>73.706800000000001</v>
+      </c>
+      <c r="C43">
+        <v>73.663899999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>72.612099999999998</v>
+      </c>
+      <c r="C44">
+        <v>74.694100000000006</v>
+      </c>
+      <c r="D44">
+        <v>77.570300000000003</v>
+      </c>
+      <c r="E44">
+        <v>79.609399999999994</v>
+      </c>
+      <c r="F44">
+        <v>79.587900000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45">
+        <v>71.088200000000001</v>
+      </c>
+      <c r="C45">
+        <v>69.864800000000002</v>
+      </c>
+      <c r="D45">
+        <v>72.826800000000006</v>
+      </c>
+      <c r="E45">
+        <v>71.925299999999993</v>
+      </c>
+      <c r="F45">
+        <v>72.719499999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46">
+        <v>74.093199999999996</v>
+      </c>
+      <c r="C46">
+        <v>73.191699999999997</v>
+      </c>
+      <c r="D46">
+        <v>75.917599999999993</v>
+      </c>
+      <c r="E46">
+        <v>76.153700000000001</v>
+      </c>
+      <c r="F46">
+        <v>76.260999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B26" xr:uid="{E840FD7A-C2C5-4D1E-BF94-872A7645ED01}">
+    <sortState ref="A2:B46">
+      <sortCondition ref="A1:A26"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E322AC-DCC3-4307-A405-E62626FABF61}">
+  <dimension ref="A1:A43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
several tests with different regexp-tokenizers
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BD843F-0A12-4D89-BAAC-5210A71C1244}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AF3AAF-65A0-4701-A14A-0E3BB834F61B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nltkClassifier" sheetId="1" r:id="rId1"/>
     <sheet name="Ideen" sheetId="2" r:id="rId2"/>
     <sheet name="Accuracy" sheetId="3" r:id="rId3"/>
-    <sheet name="ClassifierOutput" sheetId="4" r:id="rId4"/>
+    <sheet name="RandomForest" sheetId="4" r:id="rId4"/>
+    <sheet name="FilteredClassifier" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Accuracy!$A$1:$B$26</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="205">
   <si>
     <t>NaiveBayes</t>
   </si>
@@ -317,6 +318,330 @@
   </si>
   <si>
     <t xml:space="preserve">  804  465 |    b = False</t>
+  </si>
+  <si>
+    <t>all, with stopwords</t>
+  </si>
+  <si>
+    <t>Classifier Model</t>
+  </si>
+  <si>
+    <t>J48 pruned tree</t>
+  </si>
+  <si>
+    <t>------------------</t>
+  </si>
+  <si>
+    <t>COUNT(refuted) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   COUNT(blunders) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   COUNT(misses) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   COUNT(blunder.) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   COUNT(loses) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   COUNT(mistake_comma_) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   COUNT(error) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   COUNT(blunder) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   COUNT(mistake) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(too) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(allows) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(doesn_apostrophe_t) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(should) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(should_apostrophe_ve) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(costs) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(better) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(grave) = '(-inf-0.5]': True (4086.0/864.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(grave) = '(0.5-inf)': False (4.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(better) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(after) = '(-inf-0.5]': False (91.0/42.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(after) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(this) = '(-inf-0.5]': True (9.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(this) = '(0.5-inf)': False (8.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(costs) = '(0.5-inf)': False (9.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(should_apostrophe_ve) = '(0.5-inf)': False (6.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(should) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(this) = '(-inf-0.5]': False (61.0/24.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(this) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(after) = '(-inf-0.5]': True (16.0/5.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(after) = '(0.5-inf)': False (7.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(doesn_apostrophe_t) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(time) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(have) = '(-inf-0.5]': False (46.0/13.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(have) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(was) = '(-inf-0.5]': False (3.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(was) = '(0.5-inf)': True (2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(time) = '(0.5-inf)': True (3.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(allows) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(threatens) = '(-inf-0.5]': False (47.0/14.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(threatens) = '(0.5-inf)': True (2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(too) = '(0.5-inf)': False (72.0/23.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   COUNT(mistake) = '(0.5-inf)': False (22.0/5.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   COUNT(blunder) = '(0.5-inf)': False (18.0/3.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   COUNT(error) = '(0.5-inf)': False (19.0/3.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   COUNT(mistake_comma_) = '(0.5-inf)': False (10.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   COUNT(loses) = '(0.5-inf)': False (50.0/9.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   COUNT(blunder.) = '(0.5-inf)': False (16.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   COUNT(misses) = '(0.5-inf)': False (27.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   COUNT(blunders) = '(0.5-inf)': False (12.0)</t>
+  </si>
+  <si>
+    <t>COUNT(refuted) = '(0.5-inf)': False (13.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Leaves  : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size of the tree : </t>
+  </si>
+  <si>
+    <t>Attributes:   10077</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 245.86 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances        3724               79.9313 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances       935               20.0687 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.3601</t>
+  </si>
+  <si>
+    <t>Mean absolute error                      0.3007</t>
+  </si>
+  <si>
+    <t>Root mean squared error                  0.3781</t>
+  </si>
+  <si>
+    <t>Relative absolute error                 75.8559 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             84.9355 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,987    0,702    0,790      0,987    0,877      0,442    0,820     0,910     True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,298    0,013    0,896      0,298    0,447      0,442    0,820     0,696     False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Avg.    0,799    0,514    0,819      0,799    0,760      0,442    0,820     0,852     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3346   44 |    a = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  891  378 |    b = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3345   45 |    a = True</t>
+  </si>
+  <si>
+    <t>Attributes:   7229</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 184.58 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances        3770               80.9187 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances       889               19.0813 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.4005</t>
+  </si>
+  <si>
+    <t>Mean absolute error                      0.2991</t>
+  </si>
+  <si>
+    <t>Root mean squared error                  0.3731</t>
+  </si>
+  <si>
+    <t>Relative absolute error                 75.4493 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             83.8193 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,987    0,665    0,799      0,987    0,883      0,475    0,832     0,915     True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,335    0,013    0,904      0,335    0,489      0,475    0,832     0,716     False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Avg.    0,809    0,488    0,827      0,809    0,775      0,475    0,832     0,861     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  844  425 |    b = False</t>
+  </si>
+  <si>
+    <t>Bindestrich mit rein in regex oder nicht</t>
+  </si>
+  <si>
+    <t>'[\w\d-]+|[\w\.]+|\S+'</t>
+  </si>
+  <si>
+    <t>\w+|\$[\d\.]+|\S+'</t>
+  </si>
+  <si>
+    <t>Leerzeichen mit auswerten?</t>
+  </si>
+  <si>
+    <t>'[\w\d-]+|(?:\w\.)+|#[\w\d][\w\d]|\S+'</t>
+  </si>
+  <si>
+    <t>Gleichzeichen bei Umwandlung berücksichtigen</t>
+  </si>
+  <si>
+    <t>'[\w\d\-\']+|(?:\w\.)+|#[\w\d][\w\d]|\S+|\s+'</t>
+  </si>
+  <si>
+    <t>[\w\d\-\']+|(?:\w\.)+|#[\w\d][\w\d]|\S+|\s'</t>
+  </si>
+  <si>
+    <t>'(?:\w\.)+|[\w\d\-\']+|\.+|#[\w\d][\w\d]|\S+|\s+'</t>
+  </si>
+  <si>
+    <t>'(?:\w\.)+|[\w\d\-\']+|\.+|#[\w\d]{2}|1/2|[!\?]+|[\-\+/=]+|\S|\s+'</t>
+  </si>
+  <si>
+    <t>Attributes:   6365</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 129.39 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances        3748               80.4464 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances       911               19.5536 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.3784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean absolute error                      0.3   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root mean squared error                  0.374 </t>
+  </si>
+  <si>
+    <t>Relative absolute error                 75.6839 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             84.0022 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,989    0,689    0,793      0,989    0,880      0,461    0,836     0,916     True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,311    0,011    0,914      0,311    0,464      0,461    0,836     0,718     False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Avg.    0,804    0,504    0,826      0,804    0,767      0,461    0,836     0,862     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3353   37 |    a = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  874  395 |    b = False</t>
   </si>
 </sst>
 </file>
@@ -358,11 +683,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,18 +983,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -919,18 +1245,18 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1191,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74247B1C-FA49-495A-87B8-A1E34540CE36}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,6 +1563,21 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1247,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59F50FD-8FC7-422A-8F8D-928176239229}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,10 +1599,10 @@
     <col min="1" max="1" width="22.6328125" customWidth="1"/>
     <col min="2" max="2" width="7.81640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="12.7265625" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="7.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1280,8 +1621,32 @@
       <c r="F1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" t="s">
+        <v>187</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N1" t="s">
+        <v>189</v>
+      </c>
+      <c r="O1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1301,7 +1666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1320,8 +1685,11 @@
       <c r="F3">
         <v>69.177899999999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>67.052999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1340,8 +1708,11 @@
       <c r="F4">
         <v>76.303899999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>77.226900000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1352,7 +1723,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1369,7 +1740,7 @@
         <v>77.656099999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1386,7 +1757,7 @@
         <v>67.031599999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1397,12 +1768,12 @@
         <v>73.556600000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1419,7 +1790,7 @@
         <v>75.938999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1436,7 +1807,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1453,7 +1824,7 @@
         <v>77.484399999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1470,7 +1841,7 @@
         <v>77.8279</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1487,7 +1858,7 @@
         <v>75.102000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1504,7 +1875,7 @@
         <v>71.946799999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1518,7 +1889,7 @@
         <v>74.221900000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1532,7 +1903,7 @@
         <v>73.449200000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1549,7 +1920,7 @@
         <v>73.299000000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1937,7 @@
         <v>75.273700000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1577,7 +1948,7 @@
         <v>73.663899999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -1588,7 +1959,7 @@
         <v>73.127300000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
@@ -1599,7 +1970,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1618,8 +1989,11 @@
       <c r="F23">
         <v>75.617099999999994</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>76.819100000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1636,7 +2010,7 @@
         <v>75.638499999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1653,7 +2027,7 @@
         <v>75.638499999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1664,7 +2038,7 @@
         <v>73.556600000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1675,7 +2049,7 @@
         <v>73.814099999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -1692,7 +2066,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1703,7 +2077,7 @@
         <v>73.857100000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1714,7 +2088,7 @@
         <v>68.791600000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1725,7 +2099,7 @@
         <v>73.620900000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>55</v>
       </c>
@@ -1736,7 +2110,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>56</v>
       </c>
@@ -1747,7 +2121,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>57</v>
       </c>
@@ -1758,7 +2132,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1769,7 +2143,7 @@
         <v>73.556600000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1786,7 +2160,7 @@
         <v>74.415099999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1803,7 +2177,7 @@
         <v>73.213099999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -1814,7 +2188,7 @@
         <v>72.118499999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1831,7 +2205,7 @@
         <v>72.7624</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +2222,7 @@
         <v>73.299000000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1865,7 +2239,7 @@
         <v>72.633600000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -1882,7 +2256,7 @@
         <v>74.758499999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -1893,7 +2267,7 @@
         <v>73.663899999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -1912,8 +2286,35 @@
       <c r="F44">
         <v>79.587900000000005</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>79.931299999999993</v>
+      </c>
+      <c r="H44">
+        <v>80.296199999999999</v>
+      </c>
+      <c r="I44">
+        <v>80.918700000000001</v>
+      </c>
+      <c r="J44">
+        <v>80.703999999999994</v>
+      </c>
+      <c r="K44">
+        <v>80.618200000000002</v>
+      </c>
+      <c r="L44">
+        <v>80.424999999999997</v>
+      </c>
+      <c r="M44">
+        <v>79.909899999999993</v>
+      </c>
+      <c r="N44">
+        <v>80.382099999999994</v>
+      </c>
+      <c r="O44">
+        <v>80.446399999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1932,8 +2333,11 @@
       <c r="F45">
         <v>72.719499999999996</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>70.508700000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -1951,6 +2355,9 @@
       </c>
       <c r="F46">
         <v>76.260999999999996</v>
+      </c>
+      <c r="G46">
+        <v>76.4756</v>
       </c>
     </row>
   </sheetData>
@@ -1960,14 +2367,17 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E322AC-DCC3-4307-A405-E62626FABF61}">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:A177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135:A177"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2126,6 +2536,767 @@
         <v>96</v>
       </c>
     </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56662D5E-AB46-41D2-8106-7B914B0ABB00}">
+  <dimension ref="A1:B58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:B58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>152</v>
+      </c>
+      <c r="B58">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first tests with six ordinal classes
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AF3AAF-65A0-4701-A14A-0E3BB834F61B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1188685-6A80-46BE-AB5B-8F39B8994F2B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nltkClassifier" sheetId="1" r:id="rId1"/>
     <sheet name="Ideen" sheetId="2" r:id="rId2"/>
     <sheet name="Accuracy" sheetId="3" r:id="rId3"/>
-    <sheet name="RandomForest" sheetId="4" r:id="rId4"/>
-    <sheet name="FilteredClassifier" sheetId="5" r:id="rId5"/>
+    <sheet name="6 classes" sheetId="6" r:id="rId4"/>
+    <sheet name="RandomForest" sheetId="4" r:id="rId5"/>
+    <sheet name="FilteredClassifier" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Accuracy!$A$1:$B$26</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="311">
   <si>
     <t>NaiveBayes</t>
   </si>
@@ -642,6 +643,324 @@
   </si>
   <si>
     <t xml:space="preserve">  874  395 |    b = False</t>
+  </si>
+  <si>
+    <t>COUNT(blunder) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   COUNT(misses) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   COUNT(mistake) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   COUNT(error) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   COUNT(interesting) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   COUNT(loses) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   COUNT(too) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   COUNT(should) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   COUNT(better) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(refuted) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(consideration) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(_blank__carriage_return__new_line_) = '(-inf-1.5]': 2 (4060.0/1576.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(_blank__carriage_return__new_line_) = '(1.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(was) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(.) = '(-inf-0.5]': 2 (0.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(.) = '(0.5-3.5]': 2 (11.0/5.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   |   COUNT(.) = '(3.5-inf)': 5 (17.0/10.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(was) = '(0.5-inf)': 4 (8.0/4.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(consideration) = '(0.5-inf)': 3 (9.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(refuted) = '(0.5-inf)': 5 (14.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   COUNT(better) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(was) = '(-inf-0.5]': 2 (103.0/62.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(was) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(this) = '(-inf-0.5]': 4 (24.0/14.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(this) = '(0.5-inf)': 5 (14.0/8.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   COUNT(should) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   COUNT(sacrifice) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(_carriage_return__new_line_) = '(-inf-1.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(.) = '(-inf-0.5]': 3 (19.0/8.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(.) = '(0.5-3.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(this) = '(-inf-0.5]'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(was) = '(-inf-0.5]': 4 (25.0/14.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   |   COUNT(was) = '(0.5-inf)': 3 (3.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(this) = '(0.5-inf)': 5 (10.0/5.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(.) = '(3.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(better) = '(-inf-0.5]': 5 (4.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   |   COUNT(better) = '(0.5-inf)': 2 (2.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(_carriage_return__new_line_) = '(1.5-2.5]': 2 (6.0/3.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   COUNT(_carriage_return__new_line_) = '(2.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(.) = '(-inf-0.5]': 2 (0.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(.) = '(0.5-3.5]': 2 (9.0/3.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   |   |   COUNT(.) = '(3.5-inf)': 4 (4.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   COUNT(sacrifice) = '(0.5-inf)': 1 (2.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   COUNT(too) = '(0.5-inf)': 5 (85.0/49.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   COUNT(loses) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   COUNT(.) = '(-inf-0.5]': 6 (11.0/5.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   COUNT(.) = '(0.5-3.5]': 5 (30.0/15.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   COUNT(.) = '(3.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   COUNT(this) = '(-inf-0.5]': 2 (4.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   COUNT(this) = '(0.5-inf)': 3 (3.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   COUNT(interesting) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   COUNT(_blank__carriage_return__new_line_) = '(-inf-1.5]': 3 (34.0/11.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   COUNT(_blank__carriage_return__new_line_) = '(1.5-inf)': 4 (2.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   COUNT(error) = '(0.5-inf)': 5 (31.0/9.0)</t>
+  </si>
+  <si>
+    <t>|   |   COUNT(mistake) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   COUNT(better) = '(-inf-0.5]': 5 (42.0/10.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   COUNT(better) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   |   |   |   COUNT(was) = '(-inf-0.5]': 2 (3.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   COUNT(was) = '(0.5-inf)': 6 (3.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   COUNT(misses) = '(0.5-inf)': 5 (27.0/12.0)</t>
+  </si>
+  <si>
+    <t>COUNT(blunder) = '(0.5-inf)'</t>
+  </si>
+  <si>
+    <t>|   COUNT(game-losing) = '(-inf-0.5]': 5 (35.0/17.0)</t>
+  </si>
+  <si>
+    <t>|   COUNT(game-losing) = '(0.5-inf)': 6 (5.0)</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 28.05 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances        2711               58.1885 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances      1948               41.8115 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.1314</t>
+  </si>
+  <si>
+    <t>Mean absolute error                      0.2003</t>
+  </si>
+  <si>
+    <t>Root mean squared error                  0.3197</t>
+  </si>
+  <si>
+    <t>Relative absolute error                 94.2179 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             98.0835 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,000    0,001    0,000      0,000    0,000      -0,006   0,529     0,038     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,965    0,827    0,597      0,965    0,738      0,233    0,575     0,598     2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,068    0,011    0,483      0,068    0,120      0,143    0,546     0,180     3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,050    0,011    0,303      0,050    0,086      0,093    0,558     0,125     4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,183    0,036    0,467      0,183    0,263      0,223    0,592     0,276     5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,033    0,002    0,353      0,033    0,061      0,099    0,540     0,087     6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Avg.    0,582    0,471    0,507      0,582    0,477      0,194    0,569     0,415     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a    b    c    d    e    f   &lt;-- classified as</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  162    0    2    4    0 |    a = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1 2517   23   15   48    3 |    b = 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1  551   42    5   16    0 |    c = 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  326    7   20   47    0 |    d = 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2  522   11   20  126    8 |    e = 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  137    4    4   29    6 |    f = 6</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 118.92 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances        2871               61.6227 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances      1788               38.3773 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.2049</t>
+  </si>
+  <si>
+    <t>Mean absolute error                      0.1791</t>
+  </si>
+  <si>
+    <t>Root mean squared error                  0.2968</t>
+  </si>
+  <si>
+    <t>Relative absolute error                 84.2655 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             91.0506 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,000    0,001    0,000      0,000    0,000      -0,007   0,690     0,101     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,982    0,805    0,608      0,982    0,751      0,299    0,776     0,795     2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,172    0,010    0,726      0,172    0,279      0,316    0,761     0,419     3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,083    0,005    0,589      0,083    0,145      0,198    0,725     0,259     4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,179    0,016    0,661      0,179    0,281      0,295    0,787     0,458     5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0,272    0,001    0,907      0,272    0,419      0,488    0,821     0,418     6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Avg.    0,616    0,454    0,619      0,616    0,527      0,288    0,770     0,610     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  167    1    0    0    0 |    a = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6 2560   28    4    9    0 |    b = 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  506  106    2    1    0 |    c = 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  332    5   33   30    0 |    d = 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  539    5   17  123    5 |    e = 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0  107    1    0   23   49 |    f = 6</t>
   </si>
 </sst>
 </file>
@@ -1590,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59F50FD-8FC7-422A-8F8D-928176239229}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+    <sheetView topLeftCell="D37" workbookViewId="0">
       <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
@@ -2372,6 +2691,727 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5253CDD-D3CF-44E2-9B4F-B3F6AF105E31}">
+  <dimension ref="A1:B166"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:A167"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>55.956200000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>56.600099999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>58.8324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>58.188499999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>61.622700000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E322AC-DCC3-4307-A405-E62626FABF61}">
   <dimension ref="A1:A177"/>
   <sheetViews>
@@ -3006,7 +4046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56662D5E-AB46-41D2-8106-7B914B0ABB00}">
   <dimension ref="A1:B58"/>
   <sheetViews>

</xml_diff>